<commit_message>
Modifications for distance tracker
</commit_message>
<xml_diff>
--- a/flytrack_distanceTracker_settings.xlsx
+++ b/flytrack_distanceTracker_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonahpearl/Documents/MATLAB/Crickmore/FlyKnight/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ADA828B-58D8-D044-A743-3070249A4205}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600D9FCA-3EF7-1744-A569-C327B7C8EB71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6280" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5560" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flytrack_settings" sheetId="1" r:id="rId1"/>
@@ -932,7 +932,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>